<commit_message>
Update Expression Evaluation tests.xlsx
</commit_message>
<xml_diff>
--- a/Application testing/Expression Evaluation tests.xlsx
+++ b/Application testing/Expression Evaluation tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MetalUp\ILE\Application testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5344E6A-69C1-4B2A-BF8E-1112048B1768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DAC2A97-5AB3-473D-A647-DF3C7FCB155A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B12B1510-1FAF-4C1B-A606-A66F719FC9D9}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="69">
   <si>
     <t>C#</t>
   </si>
@@ -98,12 +98,6 @@
     <t>Imports System</t>
   </si>
   <si>
-    <t xml:space="preserve">new </t>
-  </si>
-  <si>
-    <t>new</t>
-  </si>
-  <si>
     <t>=   (unless   == )</t>
   </si>
   <si>
@@ -134,30 +128,18 @@
     <t>(?i)System\.</t>
   </si>
   <si>
-    <t>(?i)\sNew\s</t>
-  </si>
-  <si>
     <t>\s*print*\s*\(</t>
   </si>
   <si>
     <t>\s*input*\s*\(</t>
   </si>
   <si>
-    <t>\s*new\s</t>
-  </si>
-  <si>
     <t>\w*[^=]=[^=]</t>
   </si>
   <si>
     <t>.append</t>
   </si>
   <si>
-    <t>\snew\s\w*</t>
-  </si>
-  <si>
-    <t>NB must later permit new array i.e. new[]</t>
-  </si>
-  <si>
     <t>\.append</t>
   </si>
   <si>
@@ -165,9 +147,6 @@
   </si>
   <si>
     <t>Assignment statement (single '=') is not permitted</t>
-  </si>
-  <si>
-    <t>Assignment statement is not permitted</t>
   </si>
   <si>
     <t>Use of  {match} is not permitted</t>
@@ -244,29 +223,64 @@
     <t>Braces syntax</t>
   </si>
   <si>
-    <t>Explicit use of the System namespace is not necessary, nor permitted</t>
-  </si>
-  <si>
-    <t>'using' statements for all permissible functions are provided (invisibly). No additional 'using' statements are permitted.</t>
-  </si>
-  <si>
     <t>Use of {match}  is not permitted</t>
   </si>
   <si>
     <t>(as per C#)</t>
   </si>
   <si>
-    <t>The 'append' method  on a List is not permitted as it is a mutating method. Hint: you may use '+' to append a list to a list.</t>
-  </si>
-  <si>
     <t>\s*System(\.\w*)*</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> 'append' to a List is not permitted as it is a mutating method. Hint: you may use '+' to append a </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>list</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to a list.</t>
+    </r>
+  </si>
+  <si>
+    <t>Assignment statement (single '=') is not permitted. (If you intended to test for equality, use '==')</t>
+  </si>
+  <si>
+    <t>Assignment to a variable is not permitted</t>
+  </si>
+  <si>
+    <t>'using' statements for all permissible functions are automatically provided (behind the scenes). No additional 'using' statements are permitted.</t>
+  </si>
+  <si>
+    <t>\s(?i)imports\s\w*</t>
+  </si>
+  <si>
+    <t>'Imports' statements for all permissible functions are automatically provided (behind the scenes). No additional 'using' statements are permitted.</t>
+  </si>
+  <si>
+    <t>Explicit use of the 'System' namespace is unnecessary, and not permitted</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,6 +290,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -634,7 +656,7 @@
   <dimension ref="A1:A41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,7 +668,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -706,7 +728,7 @@
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
@@ -728,10 +750,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CA0B909-8BB4-4889-A4D7-633BF0831B74}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,10 +773,10 @@
         <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>10</v>
@@ -767,13 +789,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -781,10 +803,10 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -792,215 +814,189 @@
         <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>2</v>
+      <c r="D10" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="A11" s="2"/>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>30</v>
       </c>
-      <c r="C13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" t="s">
+      <c r="C19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" t="s">
         <v>31</v>
       </c>
-      <c r="C18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" t="s">
-        <v>19</v>
-      </c>
       <c r="D20" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="C22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24" t="s">
-        <v>71</v>
-      </c>
-      <c r="C24" t="s">
-        <v>59</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F24" t="s">
-        <v>60</v>
+      <c r="F22" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1029,17 +1025,17 @@
         <v>1</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1052,30 +1048,30 @@
         <v>0</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1083,7 +1079,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1091,10 +1087,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>